<commit_message>
added tab 19 excel template and model
</commit_message>
<xml_diff>
--- a/backend/reports/xlsx/Tab_19_rpt_PA_ActiveProjectsbyPortfolio.xlsx
+++ b/backend/reports/xlsx/Tab_19_rpt_PA_ActiveProjectsbyPortfolio.xlsx
@@ -1,20 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10709"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robrien/work/gdx-agreements-tracker/backend/reports/xlsx/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aspiteri/Development/Github/gdx-agreements-tracker/backend/reports/xlsx/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5C9F714A-8550-3C44-AD14-E14BC46BD8E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7766A7D2-A167-0B45-A831-C3DE78BA2FB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="36920" yWindow="-21100" windowWidth="21600" windowHeight="37900" xr2:uid="{FB9893AD-F19A-BB4E-A83D-FCCFB21F8723}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="26660" xr2:uid="{FB9893AD-F19A-BB4E-A83D-FCCFB21F8723}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm.Print_Titles" localSheetId="0">Sheet1!$2:$2</definedName>
+  </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -36,30 +39,96 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
-  <si>
-    <t>{#r=d.report[i]}</t>
-  </si>
-  <si>
-    <t>{#r1=d.report[i+1]}</t>
-  </si>
-  <si>
-    <t>{#t=d.report_totals[i]}</t>
-  </si>
-  <si>
-    <t>{#date=d.date}</t>
-  </si>
-  <si>
-    <t>Project #</t>
-  </si>
-  <si>
-    <t>Project Name</t>
-  </si>
-  <si>
-    <t>{#fy=d.fiscal_year}</t>
-  </si>
-  <si>
-    <t>Project ________ for {$fy} as of {$date}</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="30">
+  <si>
+    <t>#</t>
+  </si>
+  <si>
+    <t>Project Manager</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Project Type</t>
+  </si>
+  <si>
+    <t>Start Date</t>
+  </si>
+  <si>
+    <t>End Date</t>
+  </si>
+  <si>
+    <t>Planned Budget</t>
+  </si>
+  <si>
+    <t>Ministry</t>
+  </si>
+  <si>
+    <t>{$rptPrj.#}</t>
+  </si>
+  <si>
+    <t>{$rptPrj.name}</t>
+  </si>
+  <si>
+    <t>{$rptPrj.description}</t>
+  </si>
+  <si>
+    <t>{$rptPrj.project_type}</t>
+  </si>
+  <si>
+    <t>{$rptPrj.planned_budget}</t>
+  </si>
+  <si>
+    <t>{$rptPrj.ministry}</t>
+  </si>
+  <si>
+    <t>{$rptPrj1}</t>
+  </si>
+  <si>
+    <t>{#rptPrj=d.reportProjByPort[i].sectionInfo[i]}</t>
+  </si>
+  <si>
+    <t>{#rptPrj1=d.reportProjByPort[i].sectionInfo[i+1]}</t>
+  </si>
+  <si>
+    <t>{$rptPrjPort.sectionPortfolio.portfolio}</t>
+  </si>
+  <si>
+    <t>{#rptPrjPort=d.reportProjByPort[i]}</t>
+  </si>
+  <si>
+    <t>{#rptPrjPort1=d.reportProjByPort[i+1]}</t>
+  </si>
+  <si>
+    <t>{$rptPrjPort1}</t>
+  </si>
+  <si>
+    <t>{$rptPrj.start_date:formatD('DD-MMM-YY')}</t>
+  </si>
+  <si>
+    <t>{$rptPrj.end_date:formatD('DD-MMM-YY')}</t>
+  </si>
+  <si>
+    <t>Active Project Report by Portfolio</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>Report Total</t>
+  </si>
+  <si>
+    <t>{d.reportTotals.sum}</t>
+  </si>
+  <si>
+    <t>{$rptPrjPort.sectionTotal.sum}</t>
+  </si>
+  <si>
+    <t>{$rptPrj.project_manager}</t>
+  </si>
+  <si>
+    <t>‎</t>
   </si>
 </sst>
 </file>
@@ -69,7 +138,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="13">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -91,11 +160,6 @@
       <name val="BCSans-Regular"/>
     </font>
     <font>
-      <b/>
-      <sz val="8"/>
-      <name val="BCSans-Regular"/>
-    </font>
-    <font>
       <sz val="18"/>
       <color theme="0"/>
       <name val="BCSans-Regular"/>
@@ -105,8 +169,46 @@
       <color theme="1"/>
       <name val="BCSans-Regular"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF38B9C7"/>
+      <name val="Menlo"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1" tint="0.34998626667073579"/>
+      <name val="BCSans-Regular"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="BCSans-Regular"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="BCSans-Regular"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="BCSans-Regular"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1" tint="0.34998626667073579"/>
+      <name val="BCSans-Regular"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -125,8 +227,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="6">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -135,115 +249,199 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color rgb="FFBFBFBF"/>
+      <left style="thin">
+        <color theme="0"/>
       </left>
-      <right style="medium">
-        <color rgb="FFBFBFBF"/>
+      <right style="thin">
+        <color theme="0"/>
       </right>
-      <top style="medium">
-        <color rgb="FFBFBFBF"/>
+      <top style="thin">
+        <color theme="0"/>
       </top>
-      <bottom style="medium">
-        <color rgb="FFBFBFBF"/>
+      <bottom style="thin">
+        <color theme="0"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color rgb="FFBFBFBF"/>
+      <left style="thin">
+        <color theme="0"/>
       </left>
-      <right style="medium">
-        <color rgb="FFBFBFBF"/>
+      <right style="thin">
+        <color theme="0"/>
       </right>
-      <top/>
-      <bottom style="medium">
-        <color rgb="FFBFBFBF"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color rgb="FFBFBFBF"/>
-      </left>
-      <right style="medium">
-        <color rgb="FFBFBFBF"/>
-      </right>
-      <top style="medium">
-        <color rgb="FFA5A5A5"/>
+      <top style="thin">
+        <color theme="0"/>
       </top>
       <bottom/>
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
       <top/>
-      <bottom style="medium">
-        <color rgb="FFA5A5A5"/>
+      <bottom style="thin">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color theme="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
-      <right style="medium">
-        <color rgb="FFBFBFBF"/>
+      <right/>
+      <top style="thin">
+        <color theme="1"/>
+      </top>
+      <bottom style="thin">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right style="thin">
+        <color theme="0"/>
       </right>
-      <top style="medium">
-        <color rgb="FFBFBFBF"/>
-      </top>
-      <bottom style="medium">
-        <color rgb="FFBFBFBF"/>
-      </bottom>
+      <top/>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="4" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="4" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="4" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="4" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="4" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="4" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="4" fontId="10" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="4" fontId="10" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="10" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -273,15 +471,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:colOff>97692</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>48846</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>1561691</xdr:colOff>
+      <xdr:colOff>1064846</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>680356</xdr:rowOff>
+      <xdr:rowOff>561473</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -310,8 +508,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="0" y="0"/>
-          <a:ext cx="2411054" cy="680356"/>
+          <a:off x="97692" y="48846"/>
+          <a:ext cx="1817077" cy="512627"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -324,9 +522,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -364,7 +562,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -470,7 +668,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -612,7 +810,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -620,118 +818,269 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F20F7FF-D6FB-0145-BC76-92F810195548}">
-  <sheetPr>
+  <sheetPr codeName="Sheet1">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:I12"/>
+  <dimension ref="A1:I45"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="I2" sqref="C2:I2"/>
+      <pane ySplit="2" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="11.1640625" customWidth="1"/>
-    <col min="2" max="2" width="43.1640625" customWidth="1"/>
-    <col min="3" max="9" width="15.83203125" customWidth="1"/>
+    <col min="1" max="1" width="11.1640625" style="9" customWidth="1"/>
+    <col min="2" max="2" width="23.1640625" style="9" customWidth="1"/>
+    <col min="3" max="3" width="30.6640625" style="9" customWidth="1"/>
+    <col min="4" max="4" width="32.5" style="9" customWidth="1"/>
+    <col min="5" max="9" width="15.83203125" style="9" customWidth="1"/>
+    <col min="10" max="16384" width="10.83203125" style="9" hidden="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="1" customFormat="1" ht="57" customHeight="1" thickBot="1">
-      <c r="A1" s="15"/>
-      <c r="B1" s="15"/>
-      <c r="C1" s="16" t="s">
+    <row r="1" spans="1:9" s="3" customFormat="1" ht="57" customHeight="1">
+      <c r="A1" s="1"/>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="19" t="s">
+        <v>23</v>
+      </c>
+      <c r="E1" s="19"/>
+      <c r="F1" s="19"/>
+      <c r="G1" s="19"/>
+      <c r="H1" s="19"/>
+      <c r="I1" s="19"/>
+    </row>
+    <row r="2" spans="1:9" s="18" customFormat="1" ht="19">
+      <c r="A2" s="37" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="37"/>
+      <c r="C2" s="38" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="37" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="39" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" s="37" t="s">
+        <v>4</v>
+      </c>
+      <c r="G2" s="37" t="s">
+        <v>5</v>
+      </c>
+      <c r="H2" s="37" t="s">
+        <v>6</v>
+      </c>
+      <c r="I2" s="37" t="s">
         <v>7</v>
       </c>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
-      <c r="F1" s="16"/>
-      <c r="G1" s="16"/>
-      <c r="H1" s="16"/>
-      <c r="I1" s="16"/>
-    </row>
-    <row r="2" spans="1:9" s="1" customFormat="1" ht="20" thickBot="1">
-      <c r="A2" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" s="14"/>
-      <c r="D2" s="14"/>
-      <c r="E2" s="8"/>
-      <c r="F2" s="8"/>
-      <c r="G2" s="8"/>
-      <c r="H2" s="8"/>
-      <c r="I2" s="8"/>
-    </row>
-    <row r="3" spans="1:9" s="2" customFormat="1" ht="20" thickBot="1">
-      <c r="A3" s="5"/>
-      <c r="B3" s="11"/>
-      <c r="C3" s="11"/>
-      <c r="D3" s="11"/>
-      <c r="E3" s="9"/>
-      <c r="F3" s="9"/>
-      <c r="G3" s="9"/>
-      <c r="H3" s="9"/>
-      <c r="I3" s="10"/>
-    </row>
-    <row r="4" spans="1:9" s="2" customFormat="1" ht="20" thickBot="1">
-      <c r="A4" s="6"/>
-      <c r="B4" s="12"/>
-      <c r="C4" s="13"/>
-      <c r="D4" s="13"/>
-      <c r="E4" s="9"/>
-      <c r="F4" s="9"/>
-      <c r="G4" s="9"/>
-      <c r="H4" s="9"/>
-      <c r="I4" s="10"/>
-    </row>
-    <row r="5" spans="1:9" s="1" customFormat="1" ht="20" thickBot="1">
-      <c r="A5" s="3"/>
-      <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="9"/>
-      <c r="F5" s="9"/>
-      <c r="G5" s="9"/>
-      <c r="H5" s="9"/>
-      <c r="I5" s="9"/>
-    </row>
-    <row r="7" spans="1:9">
-      <c r="A7" s="4" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9">
-      <c r="A8" s="4" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9">
-      <c r="A9" s="4" t="s">
-        <v>2</v>
-      </c>
+    </row>
+    <row r="3" spans="1:9" s="5" customFormat="1" ht="19">
+      <c r="A3" s="36" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" s="4"/>
+      <c r="C3" s="7"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="8"/>
+      <c r="F3" s="7"/>
+      <c r="G3" s="7"/>
+      <c r="H3" s="7"/>
+      <c r="I3" s="7"/>
+    </row>
+    <row r="4" spans="1:9" s="17" customFormat="1" ht="19">
+      <c r="A4" s="33" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="34" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="35" t="s">
+        <v>28</v>
+      </c>
+      <c r="D4" s="34" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" s="33" t="s">
+        <v>11</v>
+      </c>
+      <c r="F4" s="33" t="s">
+        <v>21</v>
+      </c>
+      <c r="G4" s="33" t="s">
+        <v>22</v>
+      </c>
+      <c r="H4" s="33" t="s">
+        <v>12</v>
+      </c>
+      <c r="I4" s="33" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" s="14" customFormat="1" ht="19">
+      <c r="A5" s="13"/>
+      <c r="B5" s="13"/>
+      <c r="C5" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" s="15"/>
+      <c r="E5" s="15"/>
+      <c r="F5" s="16"/>
+      <c r="G5" s="16"/>
+      <c r="H5" s="16"/>
+      <c r="I5" s="16"/>
+    </row>
+    <row r="6" spans="1:9" s="24" customFormat="1">
+      <c r="A6" s="23" t="s">
+        <v>29</v>
+      </c>
+      <c r="B6" s="23" t="s">
+        <v>29</v>
+      </c>
+      <c r="C6" s="24" t="s">
+        <v>29</v>
+      </c>
+      <c r="D6" s="24" t="s">
+        <v>29</v>
+      </c>
+      <c r="E6" s="24" t="s">
+        <v>29</v>
+      </c>
+      <c r="F6" s="24" t="s">
+        <v>29</v>
+      </c>
+      <c r="G6" s="31" t="s">
+        <v>24</v>
+      </c>
+      <c r="H6" s="25" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" s="27" customFormat="1">
+      <c r="A7" s="26"/>
+      <c r="B7" s="26"/>
+      <c r="H7" s="20" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" s="29" customFormat="1">
+      <c r="A8" s="28" t="s">
+        <v>29</v>
+      </c>
+      <c r="B8" s="28" t="s">
+        <v>29</v>
+      </c>
+      <c r="C8" s="29" t="s">
+        <v>29</v>
+      </c>
+      <c r="D8" s="29" t="s">
+        <v>29</v>
+      </c>
+      <c r="E8" s="29" t="s">
+        <v>29</v>
+      </c>
+      <c r="F8" s="29" t="s">
+        <v>29</v>
+      </c>
+      <c r="G8" s="32" t="s">
+        <v>25</v>
+      </c>
+      <c r="H8" s="30" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" s="22" customFormat="1">
+      <c r="A9" s="21"/>
+      <c r="B9" s="21"/>
     </row>
     <row r="10" spans="1:9">
-      <c r="A10" s="4"/>
+      <c r="A10" s="11"/>
+      <c r="B10" s="11"/>
     </row>
     <row r="11" spans="1:9">
-      <c r="A11" s="4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9">
-      <c r="A12" s="4" t="s">
-        <v>3</v>
-      </c>
+      <c r="A11" s="11"/>
+      <c r="B11" s="11"/>
+      <c r="C11" s="10"/>
+    </row>
+    <row r="25" spans="2:3">
+      <c r="C25" s="9" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="26" spans="2:3">
+      <c r="C26" s="9" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="27" spans="2:3">
+      <c r="C27" s="9" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="28" spans="2:3">
+      <c r="C28" s="9" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="30" spans="2:3">
+      <c r="B30" s="6"/>
+      <c r="C30" s="2"/>
+    </row>
+    <row r="31" spans="2:3">
+      <c r="C31" s="12"/>
+    </row>
+    <row r="32" spans="2:3">
+      <c r="C32" s="12"/>
+    </row>
+    <row r="33" spans="3:3">
+      <c r="C33" s="12"/>
+    </row>
+    <row r="34" spans="3:3">
+      <c r="C34" s="12"/>
+    </row>
+    <row r="35" spans="3:3">
+      <c r="C35" s="12"/>
+    </row>
+    <row r="36" spans="3:3">
+      <c r="C36" s="12"/>
+    </row>
+    <row r="37" spans="3:3">
+      <c r="C37" s="12"/>
+    </row>
+    <row r="38" spans="3:3">
+      <c r="C38" s="12"/>
+    </row>
+    <row r="39" spans="3:3">
+      <c r="C39" s="12"/>
+    </row>
+    <row r="40" spans="3:3">
+      <c r="C40" s="12"/>
+    </row>
+    <row r="41" spans="3:3">
+      <c r="C41" s="12"/>
+    </row>
+    <row r="42" spans="3:3">
+      <c r="C42" s="12"/>
+    </row>
+    <row r="43" spans="3:3">
+      <c r="C43" s="12"/>
+    </row>
+    <row r="44" spans="3:3">
+      <c r="C44" s="12"/>
+    </row>
+    <row r="45" spans="3:3">
+      <c r="C45" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="C1:I1"/>
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="D1:I1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="5" scale="91" fitToHeight="0" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
+  <pageSetup paperSize="5" scale="85" fitToHeight="0" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
   <headerFooter>
     <oddFooter>&amp;LTab_43_rpt_PF_RecoveryForecast
 &amp;C&amp;P of &amp;N&amp;R{$date}</oddFooter>

</xml_diff>

<commit_message>
added tab 19 excel template and model (#740)
</commit_message>
<xml_diff>
--- a/backend/reports/xlsx/Tab_19_rpt_PA_ActiveProjectsbyPortfolio.xlsx
+++ b/backend/reports/xlsx/Tab_19_rpt_PA_ActiveProjectsbyPortfolio.xlsx
@@ -1,20 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10709"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robrien/work/gdx-agreements-tracker/backend/reports/xlsx/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aspiteri/Development/Github/gdx-agreements-tracker/backend/reports/xlsx/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5C9F714A-8550-3C44-AD14-E14BC46BD8E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7766A7D2-A167-0B45-A831-C3DE78BA2FB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="36920" yWindow="-21100" windowWidth="21600" windowHeight="37900" xr2:uid="{FB9893AD-F19A-BB4E-A83D-FCCFB21F8723}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="26660" xr2:uid="{FB9893AD-F19A-BB4E-A83D-FCCFB21F8723}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm.Print_Titles" localSheetId="0">Sheet1!$2:$2</definedName>
+  </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -36,30 +39,96 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
-  <si>
-    <t>{#r=d.report[i]}</t>
-  </si>
-  <si>
-    <t>{#r1=d.report[i+1]}</t>
-  </si>
-  <si>
-    <t>{#t=d.report_totals[i]}</t>
-  </si>
-  <si>
-    <t>{#date=d.date}</t>
-  </si>
-  <si>
-    <t>Project #</t>
-  </si>
-  <si>
-    <t>Project Name</t>
-  </si>
-  <si>
-    <t>{#fy=d.fiscal_year}</t>
-  </si>
-  <si>
-    <t>Project ________ for {$fy} as of {$date}</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="30">
+  <si>
+    <t>#</t>
+  </si>
+  <si>
+    <t>Project Manager</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Project Type</t>
+  </si>
+  <si>
+    <t>Start Date</t>
+  </si>
+  <si>
+    <t>End Date</t>
+  </si>
+  <si>
+    <t>Planned Budget</t>
+  </si>
+  <si>
+    <t>Ministry</t>
+  </si>
+  <si>
+    <t>{$rptPrj.#}</t>
+  </si>
+  <si>
+    <t>{$rptPrj.name}</t>
+  </si>
+  <si>
+    <t>{$rptPrj.description}</t>
+  </si>
+  <si>
+    <t>{$rptPrj.project_type}</t>
+  </si>
+  <si>
+    <t>{$rptPrj.planned_budget}</t>
+  </si>
+  <si>
+    <t>{$rptPrj.ministry}</t>
+  </si>
+  <si>
+    <t>{$rptPrj1}</t>
+  </si>
+  <si>
+    <t>{#rptPrj=d.reportProjByPort[i].sectionInfo[i]}</t>
+  </si>
+  <si>
+    <t>{#rptPrj1=d.reportProjByPort[i].sectionInfo[i+1]}</t>
+  </si>
+  <si>
+    <t>{$rptPrjPort.sectionPortfolio.portfolio}</t>
+  </si>
+  <si>
+    <t>{#rptPrjPort=d.reportProjByPort[i]}</t>
+  </si>
+  <si>
+    <t>{#rptPrjPort1=d.reportProjByPort[i+1]}</t>
+  </si>
+  <si>
+    <t>{$rptPrjPort1}</t>
+  </si>
+  <si>
+    <t>{$rptPrj.start_date:formatD('DD-MMM-YY')}</t>
+  </si>
+  <si>
+    <t>{$rptPrj.end_date:formatD('DD-MMM-YY')}</t>
+  </si>
+  <si>
+    <t>Active Project Report by Portfolio</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>Report Total</t>
+  </si>
+  <si>
+    <t>{d.reportTotals.sum}</t>
+  </si>
+  <si>
+    <t>{$rptPrjPort.sectionTotal.sum}</t>
+  </si>
+  <si>
+    <t>{$rptPrj.project_manager}</t>
+  </si>
+  <si>
+    <t>‎</t>
   </si>
 </sst>
 </file>
@@ -69,7 +138,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="13">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -91,11 +160,6 @@
       <name val="BCSans-Regular"/>
     </font>
     <font>
-      <b/>
-      <sz val="8"/>
-      <name val="BCSans-Regular"/>
-    </font>
-    <font>
       <sz val="18"/>
       <color theme="0"/>
       <name val="BCSans-Regular"/>
@@ -105,8 +169,46 @@
       <color theme="1"/>
       <name val="BCSans-Regular"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF38B9C7"/>
+      <name val="Menlo"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1" tint="0.34998626667073579"/>
+      <name val="BCSans-Regular"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="BCSans-Regular"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="BCSans-Regular"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="BCSans-Regular"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1" tint="0.34998626667073579"/>
+      <name val="BCSans-Regular"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -125,8 +227,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="6">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -135,115 +249,199 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color rgb="FFBFBFBF"/>
+      <left style="thin">
+        <color theme="0"/>
       </left>
-      <right style="medium">
-        <color rgb="FFBFBFBF"/>
+      <right style="thin">
+        <color theme="0"/>
       </right>
-      <top style="medium">
-        <color rgb="FFBFBFBF"/>
+      <top style="thin">
+        <color theme="0"/>
       </top>
-      <bottom style="medium">
-        <color rgb="FFBFBFBF"/>
+      <bottom style="thin">
+        <color theme="0"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color rgb="FFBFBFBF"/>
+      <left style="thin">
+        <color theme="0"/>
       </left>
-      <right style="medium">
-        <color rgb="FFBFBFBF"/>
+      <right style="thin">
+        <color theme="0"/>
       </right>
-      <top/>
-      <bottom style="medium">
-        <color rgb="FFBFBFBF"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color rgb="FFBFBFBF"/>
-      </left>
-      <right style="medium">
-        <color rgb="FFBFBFBF"/>
-      </right>
-      <top style="medium">
-        <color rgb="FFA5A5A5"/>
+      <top style="thin">
+        <color theme="0"/>
       </top>
       <bottom/>
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
       <top/>
-      <bottom style="medium">
-        <color rgb="FFA5A5A5"/>
+      <bottom style="thin">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color theme="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
-      <right style="medium">
-        <color rgb="FFBFBFBF"/>
+      <right/>
+      <top style="thin">
+        <color theme="1"/>
+      </top>
+      <bottom style="thin">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right style="thin">
+        <color theme="0"/>
       </right>
-      <top style="medium">
-        <color rgb="FFBFBFBF"/>
-      </top>
-      <bottom style="medium">
-        <color rgb="FFBFBFBF"/>
-      </bottom>
+      <top/>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="4" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="4" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="4" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="4" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="4" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="4" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="4" fontId="10" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="4" fontId="10" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="10" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -273,15 +471,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:colOff>97692</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>48846</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>1561691</xdr:colOff>
+      <xdr:colOff>1064846</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>680356</xdr:rowOff>
+      <xdr:rowOff>561473</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -310,8 +508,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="0" y="0"/>
-          <a:ext cx="2411054" cy="680356"/>
+          <a:off x="97692" y="48846"/>
+          <a:ext cx="1817077" cy="512627"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -324,9 +522,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -364,7 +562,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -470,7 +668,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -612,7 +810,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -620,118 +818,269 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F20F7FF-D6FB-0145-BC76-92F810195548}">
-  <sheetPr>
+  <sheetPr codeName="Sheet1">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:I12"/>
+  <dimension ref="A1:I45"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="I2" sqref="C2:I2"/>
+      <pane ySplit="2" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="11.1640625" customWidth="1"/>
-    <col min="2" max="2" width="43.1640625" customWidth="1"/>
-    <col min="3" max="9" width="15.83203125" customWidth="1"/>
+    <col min="1" max="1" width="11.1640625" style="9" customWidth="1"/>
+    <col min="2" max="2" width="23.1640625" style="9" customWidth="1"/>
+    <col min="3" max="3" width="30.6640625" style="9" customWidth="1"/>
+    <col min="4" max="4" width="32.5" style="9" customWidth="1"/>
+    <col min="5" max="9" width="15.83203125" style="9" customWidth="1"/>
+    <col min="10" max="16384" width="10.83203125" style="9" hidden="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="1" customFormat="1" ht="57" customHeight="1" thickBot="1">
-      <c r="A1" s="15"/>
-      <c r="B1" s="15"/>
-      <c r="C1" s="16" t="s">
+    <row r="1" spans="1:9" s="3" customFormat="1" ht="57" customHeight="1">
+      <c r="A1" s="1"/>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="19" t="s">
+        <v>23</v>
+      </c>
+      <c r="E1" s="19"/>
+      <c r="F1" s="19"/>
+      <c r="G1" s="19"/>
+      <c r="H1" s="19"/>
+      <c r="I1" s="19"/>
+    </row>
+    <row r="2" spans="1:9" s="18" customFormat="1" ht="19">
+      <c r="A2" s="37" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="37"/>
+      <c r="C2" s="38" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="37" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="39" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" s="37" t="s">
+        <v>4</v>
+      </c>
+      <c r="G2" s="37" t="s">
+        <v>5</v>
+      </c>
+      <c r="H2" s="37" t="s">
+        <v>6</v>
+      </c>
+      <c r="I2" s="37" t="s">
         <v>7</v>
       </c>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
-      <c r="F1" s="16"/>
-      <c r="G1" s="16"/>
-      <c r="H1" s="16"/>
-      <c r="I1" s="16"/>
-    </row>
-    <row r="2" spans="1:9" s="1" customFormat="1" ht="20" thickBot="1">
-      <c r="A2" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" s="14"/>
-      <c r="D2" s="14"/>
-      <c r="E2" s="8"/>
-      <c r="F2" s="8"/>
-      <c r="G2" s="8"/>
-      <c r="H2" s="8"/>
-      <c r="I2" s="8"/>
-    </row>
-    <row r="3" spans="1:9" s="2" customFormat="1" ht="20" thickBot="1">
-      <c r="A3" s="5"/>
-      <c r="B3" s="11"/>
-      <c r="C3" s="11"/>
-      <c r="D3" s="11"/>
-      <c r="E3" s="9"/>
-      <c r="F3" s="9"/>
-      <c r="G3" s="9"/>
-      <c r="H3" s="9"/>
-      <c r="I3" s="10"/>
-    </row>
-    <row r="4" spans="1:9" s="2" customFormat="1" ht="20" thickBot="1">
-      <c r="A4" s="6"/>
-      <c r="B4" s="12"/>
-      <c r="C4" s="13"/>
-      <c r="D4" s="13"/>
-      <c r="E4" s="9"/>
-      <c r="F4" s="9"/>
-      <c r="G4" s="9"/>
-      <c r="H4" s="9"/>
-      <c r="I4" s="10"/>
-    </row>
-    <row r="5" spans="1:9" s="1" customFormat="1" ht="20" thickBot="1">
-      <c r="A5" s="3"/>
-      <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="9"/>
-      <c r="F5" s="9"/>
-      <c r="G5" s="9"/>
-      <c r="H5" s="9"/>
-      <c r="I5" s="9"/>
-    </row>
-    <row r="7" spans="1:9">
-      <c r="A7" s="4" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9">
-      <c r="A8" s="4" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9">
-      <c r="A9" s="4" t="s">
-        <v>2</v>
-      </c>
+    </row>
+    <row r="3" spans="1:9" s="5" customFormat="1" ht="19">
+      <c r="A3" s="36" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" s="4"/>
+      <c r="C3" s="7"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="8"/>
+      <c r="F3" s="7"/>
+      <c r="G3" s="7"/>
+      <c r="H3" s="7"/>
+      <c r="I3" s="7"/>
+    </row>
+    <row r="4" spans="1:9" s="17" customFormat="1" ht="19">
+      <c r="A4" s="33" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="34" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="35" t="s">
+        <v>28</v>
+      </c>
+      <c r="D4" s="34" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" s="33" t="s">
+        <v>11</v>
+      </c>
+      <c r="F4" s="33" t="s">
+        <v>21</v>
+      </c>
+      <c r="G4" s="33" t="s">
+        <v>22</v>
+      </c>
+      <c r="H4" s="33" t="s">
+        <v>12</v>
+      </c>
+      <c r="I4" s="33" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" s="14" customFormat="1" ht="19">
+      <c r="A5" s="13"/>
+      <c r="B5" s="13"/>
+      <c r="C5" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" s="15"/>
+      <c r="E5" s="15"/>
+      <c r="F5" s="16"/>
+      <c r="G5" s="16"/>
+      <c r="H5" s="16"/>
+      <c r="I5" s="16"/>
+    </row>
+    <row r="6" spans="1:9" s="24" customFormat="1">
+      <c r="A6" s="23" t="s">
+        <v>29</v>
+      </c>
+      <c r="B6" s="23" t="s">
+        <v>29</v>
+      </c>
+      <c r="C6" s="24" t="s">
+        <v>29</v>
+      </c>
+      <c r="D6" s="24" t="s">
+        <v>29</v>
+      </c>
+      <c r="E6" s="24" t="s">
+        <v>29</v>
+      </c>
+      <c r="F6" s="24" t="s">
+        <v>29</v>
+      </c>
+      <c r="G6" s="31" t="s">
+        <v>24</v>
+      </c>
+      <c r="H6" s="25" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" s="27" customFormat="1">
+      <c r="A7" s="26"/>
+      <c r="B7" s="26"/>
+      <c r="H7" s="20" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" s="29" customFormat="1">
+      <c r="A8" s="28" t="s">
+        <v>29</v>
+      </c>
+      <c r="B8" s="28" t="s">
+        <v>29</v>
+      </c>
+      <c r="C8" s="29" t="s">
+        <v>29</v>
+      </c>
+      <c r="D8" s="29" t="s">
+        <v>29</v>
+      </c>
+      <c r="E8" s="29" t="s">
+        <v>29</v>
+      </c>
+      <c r="F8" s="29" t="s">
+        <v>29</v>
+      </c>
+      <c r="G8" s="32" t="s">
+        <v>25</v>
+      </c>
+      <c r="H8" s="30" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" s="22" customFormat="1">
+      <c r="A9" s="21"/>
+      <c r="B9" s="21"/>
     </row>
     <row r="10" spans="1:9">
-      <c r="A10" s="4"/>
+      <c r="A10" s="11"/>
+      <c r="B10" s="11"/>
     </row>
     <row r="11" spans="1:9">
-      <c r="A11" s="4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9">
-      <c r="A12" s="4" t="s">
-        <v>3</v>
-      </c>
+      <c r="A11" s="11"/>
+      <c r="B11" s="11"/>
+      <c r="C11" s="10"/>
+    </row>
+    <row r="25" spans="2:3">
+      <c r="C25" s="9" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="26" spans="2:3">
+      <c r="C26" s="9" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="27" spans="2:3">
+      <c r="C27" s="9" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="28" spans="2:3">
+      <c r="C28" s="9" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="30" spans="2:3">
+      <c r="B30" s="6"/>
+      <c r="C30" s="2"/>
+    </row>
+    <row r="31" spans="2:3">
+      <c r="C31" s="12"/>
+    </row>
+    <row r="32" spans="2:3">
+      <c r="C32" s="12"/>
+    </row>
+    <row r="33" spans="3:3">
+      <c r="C33" s="12"/>
+    </row>
+    <row r="34" spans="3:3">
+      <c r="C34" s="12"/>
+    </row>
+    <row r="35" spans="3:3">
+      <c r="C35" s="12"/>
+    </row>
+    <row r="36" spans="3:3">
+      <c r="C36" s="12"/>
+    </row>
+    <row r="37" spans="3:3">
+      <c r="C37" s="12"/>
+    </row>
+    <row r="38" spans="3:3">
+      <c r="C38" s="12"/>
+    </row>
+    <row r="39" spans="3:3">
+      <c r="C39" s="12"/>
+    </row>
+    <row r="40" spans="3:3">
+      <c r="C40" s="12"/>
+    </row>
+    <row r="41" spans="3:3">
+      <c r="C41" s="12"/>
+    </row>
+    <row r="42" spans="3:3">
+      <c r="C42" s="12"/>
+    </row>
+    <row r="43" spans="3:3">
+      <c r="C43" s="12"/>
+    </row>
+    <row r="44" spans="3:3">
+      <c r="C44" s="12"/>
+    </row>
+    <row r="45" spans="3:3">
+      <c r="C45" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="C1:I1"/>
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="D1:I1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="5" scale="91" fitToHeight="0" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
+  <pageSetup paperSize="5" scale="85" fitToHeight="0" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
   <headerFooter>
     <oddFooter>&amp;LTab_43_rpt_PF_RecoveryForecast
 &amp;C&amp;P of &amp;N&amp;R{$date}</oddFooter>

</xml_diff>